<commit_message>
fixed one cell in rq1-3 variable definitions
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28103"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5358931-3586-45B9-82F0-F73BDE4D8481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EC6242B-1541-4EE8-86B3-8491767CE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
     <t>Levels</t>
   </si>
   <si>
-    <t>1-4 : Order 1 - Kitware - ADEPT MJ; Parallax - ST QoL; Parallax - ADEPT IG; Kitware - ST VoL \n Order 2 - Kitware - ST QoL; Kitware - ADEPT IG; Parallax - ST VoL; Parallax - ADEPT MJ \n Order 3 - Parallax - ADEPT MJ; Parallax - ST QoL; Kitware - ADEPT IG; Kitware - ST VoL \n Order 4 - Parallax - ST VoL; Kitware - ST QoL; Parallax - ADEPT IG; Kitware - ADEPT MJ</t>
+    <t>1-4 \n Order 1 - Kitware - ADEPT MJ; Parallax - ST QoL; Parallax - ADEPT IG; Kitware - ST VoL \n Order 2 - Kitware - ST QoL; Kitware - ADEPT IG; Parallax - ST VoL; Parallax - ADEPT MJ \n Order 3 - Parallax - ADEPT MJ; Parallax - ST QoL; Kitware - ADEPT IG; Kitware - ST VoL \n Order 4 - Parallax - ST VoL; Kitware - ST QoL; Parallax - ADEPT IG; Kitware - ADEPT MJ</t>
   </si>
   <si>
     <t>Military or civilian</t>
@@ -577,7 +577,7 @@
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
updated variable definitions to include session ids
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28116"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EC6242B-1541-4EE8-86B3-8491767CE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EE7BC46-F7E6-4FD4-914D-F18A51AE0894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>Variables</t>
   </si>
@@ -75,6 +75,9 @@
     <t>Alignment score (Delegator|target)</t>
   </si>
   <si>
+    <t>Server Session ID (Delegator)</t>
+  </si>
+  <si>
     <t>ADM_Aligned_Status (Baseline/Misaligned/Aligned)</t>
   </si>
   <si>
@@ -114,6 +117,9 @@
     <t>TA1 server via Delegation survey loading log</t>
   </si>
   <si>
+    <t>Text Scenario Output/TA1 server</t>
+  </si>
+  <si>
     <t>TA1 server post experiment</t>
   </si>
   <si>
@@ -145,6 +151,9 @@
   </si>
   <si>
     <t>Calculated alignment score between the KDMA measurement of a delegator and a target</t>
+  </si>
+  <si>
+    <t>The session id used to get the delegator's alignment score from the TA1 server for the text scenarios</t>
   </si>
   <si>
     <t>Assigned to the presented ADM based on baseline vs. aligned; and then based on the alignment score between the delegator and the target where aligned is the most aligned and misaligned is the least aligned (see exceptions)</t>
@@ -574,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -585,7 +594,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="121.5">
+    <row r="1" spans="1:24" ht="121.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,203 +664,212 @@
       <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" ht="91.5">
+    <row r="2" spans="1:24" ht="91.5">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="409.6">
+    <row r="3" spans="1:24" ht="409.6">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="409.6">
+    <row r="4" spans="1:24" ht="409.6">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>59</v>
+      <c r="S4" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished adding filters to RQ pages
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28116"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EE7BC46-F7E6-4FD4-914D-F18A51AE0894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61E2F591-C7BD-405E-887F-96D1406B86B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>Variables</t>
   </si>
@@ -45,6 +45,9 @@
     <t>Delegator_grp</t>
   </si>
   <si>
+    <t>Delegator_mil</t>
+  </si>
+  <si>
     <t>Delegator_Role</t>
   </si>
   <si>
@@ -132,6 +135,9 @@
     <t>Used to track and identify participants, also called participant ID</t>
   </si>
   <si>
+    <t>Does this individual have a military background?</t>
+  </si>
+  <si>
     <t>Professional medical role</t>
   </si>
   <si>
@@ -181,6 +187,9 @@
   </si>
   <si>
     <t>Military or civilian</t>
+  </si>
+  <si>
+    <t>yes or no</t>
   </si>
   <si>
     <t>EMT, paramedic, resident, physician, or other</t>
@@ -583,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -594,7 +603,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="121.5">
+    <row r="1" spans="1:25" ht="121.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,209 +676,221 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" ht="91.5">
+    <row r="2" spans="1:25" ht="91.5">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="409.6">
+    <row r="3" spans="1:25" ht="409.6">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="M3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="X3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="409.6">
+    <row r="4" spans="1:25" ht="409.6">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="K4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="S4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>62</v>
+      <c r="T4" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
setup for sim/adm alignment comparison
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28116"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61E2F591-C7BD-405E-887F-96D1406B86B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FF48BA3-5FBA-47AD-A970-95F90368B44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>Variables</t>
   </si>
@@ -78,6 +78,9 @@
     <t>Alignment score (Delegator|target)</t>
   </si>
   <si>
+    <t>Alignment score (Participant_sim|Observed_ADM(target))</t>
+  </si>
+  <si>
     <t>Server Session ID (Delegator)</t>
   </si>
   <si>
@@ -120,6 +123,9 @@
     <t>TA1 server via Delegation survey loading log</t>
   </si>
   <si>
+    <t>TA1 server Post Experiment</t>
+  </si>
+  <si>
     <t>Text Scenario Output/TA1 server</t>
   </si>
   <si>
@@ -157,6 +163,9 @@
   </si>
   <si>
     <t>Calculated alignment score between the KDMA measurement of a delegator and a target</t>
+  </si>
+  <si>
+    <t>Compares the KDMA measurement based on participant probe responses in the simulated scenario to an ADM they observed in the delegation survey</t>
   </si>
   <si>
     <t>The session id used to get the delegator's alignment score from the TA1 server for the text scenarios</t>
@@ -238,13 +247,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -267,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -276,6 +290,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -592,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -603,7 +620,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="121.5">
+    <row r="1" spans="1:26" ht="121.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +666,7 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -679,218 +696,230 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" ht="91.5">
+    <row r="2" spans="1:26" ht="91.5">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="W2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="409.6">
+    <row r="3" spans="1:26" ht="409.6">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.6">
+    <row r="4" spans="1:26" ht="409.6">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>65</v>
+      <c r="U4" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed missing rq1 data
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28415"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FF48BA3-5FBA-47AD-A970-95F90368B44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48C655C4-1360-48D2-A460-F53856E5910B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
   <si>
     <t>Variables</t>
   </si>
@@ -90,6 +90,9 @@
     <t>ADM Loading</t>
   </si>
   <si>
+    <t>Competence Error</t>
+  </si>
+  <si>
     <t>Alignment score (Delegator|Observed_ADM (target))</t>
   </si>
   <si>
@@ -177,6 +180,9 @@
     <t>Exceptions are noted when the presented ADM was not the most aligned or least aligned. This occurs in cases when the baseline matched the most aligned or where either the baseline or the aligned matched the least aligned.</t>
   </si>
   <si>
+    <t>During the Phase 1 experiment, several kitware aligned targets had competence errors. This column shows which participants experienced that error in the delegation survey</t>
+  </si>
+  <si>
     <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey</t>
   </si>
   <si>
@@ -232,6 +238,9 @@
   </si>
   <si>
     <t>Normal or Exception</t>
+  </si>
+  <si>
+    <t>1 for competence error, 0 for none</t>
   </si>
   <si>
     <t>1-5</t>
@@ -609,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,7 +629,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="121.5">
+    <row r="1" spans="1:27" ht="121.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,227 +708,239 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" ht="91.5">
+    <row r="2" spans="1:27" ht="91.5">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="409.6">
+    <row r="3" spans="1:27" ht="409.6">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="Z3" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="409.6">
+    <row r="4" spans="1:27" ht="409.6">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="S4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>68</v>
+      <c r="V4" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
do not call out team in definitions
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ1_RQ3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28415"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48C655C4-1360-48D2-A460-F53856E5910B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8CE950D-8CB5-4A6F-922A-D7136CCAB88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
     <t>Exceptions are noted when the presented ADM was not the most aligned or least aligned. This occurs in cases when the baseline matched the most aligned or where either the baseline or the aligned matched the least aligned.</t>
   </si>
   <si>
-    <t>During the Phase 1 experiment, several kitware aligned targets had competence errors. This column shows which participants experienced that error in the delegation survey</t>
+    <t>During the Phase 1 experiment, several ADMs had competence errors. This column shows which participants experienced one of those errors in the delegation survey</t>
   </si>
   <si>
     <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey</t>
@@ -621,7 +621,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>